<commit_message>
pushing originamility of the third portion
</commit_message>
<xml_diff>
--- a/docs/sheet.xlsx
+++ b/docs/sheet.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DONKAMS\Downloads\brownway-food-solutions\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D291383-E956-46BF-88E2-ED7B6E0AD275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB720112-A879-4B1F-B46F-BC55974C4801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Start-Up Costs" sheetId="1" r:id="rId1"/>
+    <sheet name="Revenue Analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="Revenue Projection" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="106">
   <si>
     <t>Item</t>
   </si>
@@ -172,6 +174,177 @@
   </si>
   <si>
     <t>Profit per Customer (LTV)</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Monthly Revenue (£)</t>
+  </si>
+  <si>
+    <t>Cumulative Revenue (£)</t>
+  </si>
+  <si>
+    <t>Total Annual Revenue from Regular Sales</t>
+  </si>
+  <si>
+    <t>Monthly Subscribers</t>
+  </si>
+  <si>
+    <t>Total Annual Revenue from Subscription Model</t>
+  </si>
+  <si>
+    <t>Total Annual Revenue (£)</t>
+  </si>
+  <si>
+    <t>Revenue from Regular Sales</t>
+  </si>
+  <si>
+    <t>Revenue from Subscription Model</t>
+  </si>
+  <si>
+    <t>Revenue from Bulk Sales</t>
+  </si>
+  <si>
+    <t>Total Annual Revenue</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>KANO Attribute</t>
+  </si>
+  <si>
+    <t>Essential Nutrients</t>
+  </si>
+  <si>
+    <t>Must-be</t>
+  </si>
+  <si>
+    <t>Easy Preparation</t>
+  </si>
+  <si>
+    <t>High-quality Taste</t>
+  </si>
+  <si>
+    <t>One-dimensional</t>
+  </si>
+  <si>
+    <t>Convenient Packaging</t>
+  </si>
+  <si>
+    <t>Affordable Pricing</t>
+  </si>
+  <si>
+    <t>Long Shelf Life</t>
+  </si>
+  <si>
+    <t>Variety of Flavors</t>
+  </si>
+  <si>
+    <t>Attractive</t>
+  </si>
+  <si>
+    <t>Cultural Stories on Packaging</t>
+  </si>
+  <si>
+    <t>Eco-friendly Packaging</t>
+  </si>
+  <si>
+    <t>Customizable Recipes</t>
+  </si>
+  <si>
+    <t>Packaging Color</t>
+  </si>
+  <si>
+    <t>Indifferent</t>
+  </si>
+  <si>
+    <t>Brand Logo Placement</t>
+  </si>
+  <si>
+    <t>Overly Spicy Options</t>
+  </si>
+  <si>
+    <t>Reverse</t>
+  </si>
+  <si>
+    <t>Complex Recipe Suggestions</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Monthly Sales (Units)</t>
+  </si>
+  <si>
+    <t>Unit Price (£)</t>
+  </si>
+  <si>
+    <t>Annual Revenue (£)</t>
+  </si>
+  <si>
+    <t>Supermarkets</t>
+  </si>
+  <si>
+    <t>Specialty Food Stores</t>
+  </si>
+  <si>
+    <t>E-commerce Website</t>
+  </si>
+  <si>
+    <t>Third-party Platforms</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Subscription Type</t>
+  </si>
+  <si>
+    <t>Monthly Fee (£)</t>
+  </si>
+  <si>
+    <t>Monthly Subscription Boxes</t>
+  </si>
+  <si>
+    <t>Quarterly Subscription Boxes</t>
+  </si>
+  <si>
+    <t>7,000 (quarterly)</t>
+  </si>
+  <si>
+    <t>5,000 + 7,000/3</t>
+  </si>
+  <si>
+    <t>60,000 + 28,000</t>
+  </si>
+  <si>
+    <t>Monthly Orders</t>
+  </si>
+  <si>
+    <t>Order Size (Units)</t>
+  </si>
+  <si>
+    <t>Restaurants/Caterers</t>
+  </si>
+  <si>
+    <t>Schools/Universities</t>
+  </si>
+  <si>
+    <t>Revenue Stream</t>
+  </si>
+  <si>
+    <t>Direct Product Sales</t>
+  </si>
+  <si>
+    <t>Subscription Services</t>
+  </si>
+  <si>
+    <t>Bulk Sales and Partnerships</t>
+  </si>
+  <si>
+    <t>Total Projected Revenue</t>
   </si>
 </sst>
 </file>
@@ -244,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -276,65 +449,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="59">
     <dxf>
       <font>
         <b/>
@@ -353,16 +481,121 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -410,6 +643,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -429,6 +687,86 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -455,13 +793,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -591,6 +922,77 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -605,95 +1007,196 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9525C1B0-10F5-46F4-AC12-C0C392BB79A8}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9525C1B0-10F5-46F4-AC12-C0C392BB79A8}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="58">
   <autoFilter ref="A1:B6" xr:uid="{9525C1B0-10F5-46F4-AC12-C0C392BB79A8}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9C69E967-FB34-436F-A6C0-E16ACBB06421}" name="Item" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{BD8E83C4-8FB1-4C53-B652-FD2D00CCB6A3}" name="Cost (£)" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{9C69E967-FB34-436F-A6C0-E16ACBB06421}" name="Item" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{BD8E83C4-8FB1-4C53-B652-FD2D00CCB6A3}" name="Cost (£)" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A3CFDF8-3E8A-400F-89BA-AFC3E5573BA4}" name="Table10" displayName="Table10" ref="M19:N26" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6A3CFDF8-3E8A-400F-89BA-AFC3E5573BA4}" name="Table10" displayName="Table10" ref="M19:N26" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="M19:N26" xr:uid="{6A3CFDF8-3E8A-400F-89BA-AFC3E5573BA4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00050F21-8A46-4700-89F9-76B0CB31A029}" name="Metric" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{C88F2753-EB10-4A50-A141-59B4D589E9B4}" name="Value (£)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00050F21-8A46-4700-89F9-76B0CB31A029}" name="Metric" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{C88F2753-EB10-4A50-A141-59B4D589E9B4}" name="Value (£)" dataDxfId="29"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F2D737E4-9C58-41D6-9601-824550290624}" name="Table11" displayName="Table11" ref="A1:C14" totalsRowShown="0" headerRowDxfId="28">
+  <autoFilter ref="A1:C14" xr:uid="{F2D737E4-9C58-41D6-9601-824550290624}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B1DF5747-516C-4DC4-9BFC-C2ADE0B29AE8}" name="Month" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{53D7CDD4-5114-4840-B6C5-A0AE42682A93}" name="Monthly Revenue (£)" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{E4FCE16C-55D8-4FF6-9E11-4D1EA7527AAB}" name="Cumulative Revenue (£)" dataDxfId="27"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D2540750-2D7B-47BD-AEF7-8E62D1BFFDC2}" name="Table12" displayName="Table12" ref="E1:H14" totalsRowShown="0" headerRowDxfId="20">
+  <autoFilter ref="E1:H14" xr:uid="{D2540750-2D7B-47BD-AEF7-8E62D1BFFDC2}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3701FD56-2A3D-4ACE-98B0-1ED602C25C90}" name="Month" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{E70D78EC-CDD5-4197-A0D2-4DB681D685CF}" name="Monthly Subscribers" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{83186F90-3647-4DCB-893B-91A2A1B84978}" name="Monthly Revenue (£)" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{E115D264-56FB-453C-A4BD-0D432C9DE5AF}" name="Cumulative Revenue (£)" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7DE8EA25-9476-4042-B537-39F8CBB33E67}" name="Table13" displayName="Table13" ref="J32:K36" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="J32:K36" xr:uid="{7DE8EA25-9476-4042-B537-39F8CBB33E67}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6733BF08-BFFE-4175-ADE7-019802123D96}" name="Category" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{7B212A16-0A4C-4ECB-AB7A-BFE2F278EF6B}" name="Total Annual Revenue (£)" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{EA8C73B8-05EA-4945-829C-5DAB49248346}" name="Table14" displayName="Table14" ref="A38:B52" totalsRowShown="0" headerRowDxfId="13" dataDxfId="14">
+  <autoFilter ref="A38:B52" xr:uid="{EA8C73B8-05EA-4945-829C-5DAB49248346}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{F12BAA1C-D500-4323-A38A-3E0530B07C25}" name="Feature" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{FA273061-24BA-4D16-A221-03070625A9C5}" name="KANO Attribute" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{F14E1B5F-CEED-4E8A-9B6B-7057A5548D51}" name="Table15" displayName="Table15" ref="A1:E6" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:E6" xr:uid="{F14E1B5F-CEED-4E8A-9B6B-7057A5548D51}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{568C35A6-69CA-4B21-959C-BF4E933A41D0}" name="Channel" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{67BCFAE2-A3EE-4263-BDD4-7EEF7ADB4557}" name="Monthly Sales (Units)"/>
+    <tableColumn id="3" xr3:uid="{AEB079EE-D7BE-4F72-8F22-A8E2B638B837}" name="Unit Price (£)" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{A093ED16-755F-47AD-A8A7-91B936186879}" name="Monthly Revenue (£)" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{7739683D-6DEC-44DE-81F9-B598F0E4EFFD}" name="Annual Revenue (£)" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{C4934AF7-E884-4702-A3DF-4B29C110DB0F}" name="Table16" displayName="Table16" ref="H1:L4" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="H1:L4" xr:uid="{C4934AF7-E884-4702-A3DF-4B29C110DB0F}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{BB916D80-DE62-4CB5-B5C0-8B50530F296D}" name="Subscription Type"/>
+    <tableColumn id="2" xr3:uid="{63C75D72-DA1A-48C0-9831-EF5DB8AC00CF}" name="Monthly Subscribers"/>
+    <tableColumn id="3" xr3:uid="{C365E1CA-A6A9-4C3C-A3EF-8709E4423149}" name="Monthly Fee (£)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{39F39BC3-D836-490C-8F38-7DE996E4DF5E}" name="Monthly Revenue (£)"/>
+    <tableColumn id="5" xr3:uid="{10E98402-80DE-4866-BB06-36904EA86160}" name="Annual Revenue (£)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{034521ED-CA6E-40AD-A93B-CAB4E6928A76}" name="Table17" displayName="Table17" ref="O1:T4" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="O1:T4" xr:uid="{034521ED-CA6E-40AD-A93B-CAB4E6928A76}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{1E3F2EAA-4F02-4675-BF71-475145206D00}" name="Channel"/>
+    <tableColumn id="2" xr3:uid="{DF59AE60-13D0-4635-83F9-6D89F6C919E3}" name="Monthly Orders"/>
+    <tableColumn id="3" xr3:uid="{3A85E5E3-8B32-4E81-8097-100FE33805C5}" name="Order Size (Units)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{3552DA32-67F0-44FB-81AB-FD370D73DF98}" name="Unit Price (£)" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{25A60996-3088-4EDF-8F9F-0629D89FD93D}" name="Monthly Revenue (£)"/>
+    <tableColumn id="6" xr3:uid="{03C19A9C-3407-4180-A9D0-0DEC1D07859A}" name="Annual Revenue (£)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{216359F1-681A-4BCD-8F7B-22CC0CEDA0C5}" name="Table18" displayName="Table18" ref="A11:B15" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A11:B15" xr:uid="{216359F1-681A-4BCD-8F7B-22CC0CEDA0C5}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{2EFE4E4D-1154-43C6-AC9C-3E5A30216CDE}" name="Revenue Stream" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E1F6216E-C226-4A3C-8FBA-013A1585C705}" name="Annual Revenue (£)" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{127B55B3-17C9-41B9-A96A-D04B39FE68EE}" name="Table2" displayName="Table2" ref="E1:F7" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{127B55B3-17C9-41B9-A96A-D04B39FE68EE}" name="Table2" displayName="Table2" ref="E1:F7" totalsRowShown="0" headerRowDxfId="55">
   <autoFilter ref="E1:F7" xr:uid="{127B55B3-17C9-41B9-A96A-D04B39FE68EE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{10489480-C599-4E2D-BE4D-35A33C2CE029}" name="Item" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{165372B0-6E7F-499C-AB80-1481C48CEF04}" name="Cost (£)" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{10489480-C599-4E2D-BE4D-35A33C2CE029}" name="Item" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{165372B0-6E7F-499C-AB80-1481C48CEF04}" name="Cost (£)" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C815F15F-3413-45AC-8F30-CE59FC9A9A1F}" name="Table3" displayName="Table3" ref="I1:J5" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C815F15F-3413-45AC-8F30-CE59FC9A9A1F}" name="Table3" displayName="Table3" ref="I1:J5" totalsRowShown="0" headerRowDxfId="52">
   <autoFilter ref="I1:J5" xr:uid="{C815F15F-3413-45AC-8F30-CE59FC9A9A1F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{055B7DF6-F220-4B82-A711-5DF52DE0CCDE}" name="Item" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{A626A692-FA63-4E67-A467-02F173ED820A}" name="Cost (£)" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{055B7DF6-F220-4B82-A711-5DF52DE0CCDE}" name="Item" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{A626A692-FA63-4E67-A467-02F173ED820A}" name="Cost (£)" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0D389971-6275-4492-9485-2B0691EC3901}" name="Table4" displayName="Table4" ref="M1:N5" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0D389971-6275-4492-9485-2B0691EC3901}" name="Table4" displayName="Table4" ref="M1:N5" totalsRowShown="0" headerRowDxfId="49">
   <autoFilter ref="M1:N5" xr:uid="{0D389971-6275-4492-9485-2B0691EC3901}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{88A9863A-778E-4C6F-AF66-DCDC5EF597B9}" name="Item" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{75FD10F3-9F75-4C44-A3ED-DA20853F4C18}" name="Cost (£)" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{88A9863A-778E-4C6F-AF66-DCDC5EF597B9}" name="Item" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{75FD10F3-9F75-4C44-A3ED-DA20853F4C18}" name="Cost (£)" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{94E49222-F96B-4B0E-8E28-2C40E9AFEB71}" name="Table5" displayName="Table5" ref="A10:B15" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{94E49222-F96B-4B0E-8E28-2C40E9AFEB71}" name="Table5" displayName="Table5" ref="A10:B15" totalsRowShown="0" headerRowDxfId="46">
   <autoFilter ref="A10:B15" xr:uid="{94E49222-F96B-4B0E-8E28-2C40E9AFEB71}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{556014DE-ECDB-42B4-9BB8-045B4D723A8D}" name="Item" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{CE9C88E0-87AC-436D-A4DF-CC9DF7594252}" name="Cost (£)" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{556014DE-ECDB-42B4-9BB8-045B4D723A8D}" name="Item" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{CE9C88E0-87AC-436D-A4DF-CC9DF7594252}" name="Cost (£)" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C9ED4651-6DCE-4881-BB42-3BFEF73DF963}" name="Table6" displayName="Table6" ref="E10:F15" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C9ED4651-6DCE-4881-BB42-3BFEF73DF963}" name="Table6" displayName="Table6" ref="E10:F15" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="E10:F15" xr:uid="{C9ED4651-6DCE-4881-BB42-3BFEF73DF963}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A8BD56F1-8966-499F-BBC4-9D70FC9991C7}" name="Item" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{88E8246C-F8D7-427D-A72A-4E69F6E4CA48}" name="Cost (£)" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{A8BD56F1-8966-499F-BBC4-9D70FC9991C7}" name="Item" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{88E8246C-F8D7-427D-A72A-4E69F6E4CA48}" name="Cost (£)" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CE3D71FA-10B6-4A92-BF2D-45D453A6CABE}" name="Table7" displayName="Table7" ref="I10:J15" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CE3D71FA-10B6-4A92-BF2D-45D453A6CABE}" name="Table7" displayName="Table7" ref="I10:J15" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="I10:J15" xr:uid="{CE3D71FA-10B6-4A92-BF2D-45D453A6CABE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C5DA9413-2F30-4B83-8408-5C94D6F60349}" name="Item" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{04ECAAD2-EAD6-4E9E-A31F-A16C32A2AB81}" name="Cost (£)" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{C5DA9413-2F30-4B83-8408-5C94D6F60349}" name="Item" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{04ECAAD2-EAD6-4E9E-A31F-A16C32A2AB81}" name="Cost (£)" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{626D2FA9-2D1A-488E-8614-157123D3FEF8}" name="Table8" displayName="Table8" ref="M10:N12" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{626D2FA9-2D1A-488E-8614-157123D3FEF8}" name="Table8" displayName="Table8" ref="M10:N12" totalsRowShown="0" headerRowDxfId="37">
   <autoFilter ref="M10:N12" xr:uid="{626D2FA9-2D1A-488E-8614-157123D3FEF8}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{9297D6E0-537A-466E-B5A6-2E943359A5FE}" name="Item"/>
@@ -704,11 +1207,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{EEAD56E5-BEA2-40E1-B366-A217AB71D0AE}" name="Table9" displayName="Table9" ref="A18:B27" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{EEAD56E5-BEA2-40E1-B366-A217AB71D0AE}" name="Table9" displayName="Table9" ref="A18:B27" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="A18:B27" xr:uid="{EEAD56E5-BEA2-40E1-B366-A217AB71D0AE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D9F416E0-9EB8-4D47-9CFF-23D8CA830FEB}" name="Category" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8EE3DD3D-E82F-4E17-84F8-BBE562606910}" name="Cost (£)" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{D9F416E0-9EB8-4D47-9CFF-23D8CA830FEB}" name="Category" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{8EE3DD3D-E82F-4E17-84F8-BBE562606910}" name="Cost (£)" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -979,7 +1482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -1401,7 +1904,7 @@
       <c r="M26" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="N26" s="11">
+      <c r="N26" s="4">
         <v>3</v>
       </c>
     </row>
@@ -1429,4 +1932,817 @@
     <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB62A7D-8AEC-48CC-B617-CCF125D6819A}">
+  <dimension ref="A1:K52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:B52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>15000</v>
+      </c>
+      <c r="C2" s="12">
+        <v>15000</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11">
+        <v>200</v>
+      </c>
+      <c r="G2" s="12">
+        <v>2400</v>
+      </c>
+      <c r="H2" s="12">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
+        <v>16500</v>
+      </c>
+      <c r="C3" s="12">
+        <v>31500</v>
+      </c>
+      <c r="E3" s="11">
+        <v>2</v>
+      </c>
+      <c r="F3" s="11">
+        <v>220</v>
+      </c>
+      <c r="G3" s="12">
+        <v>2640</v>
+      </c>
+      <c r="H3" s="12">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>18150</v>
+      </c>
+      <c r="C4" s="12">
+        <v>49650</v>
+      </c>
+      <c r="E4" s="11">
+        <v>3</v>
+      </c>
+      <c r="F4" s="11">
+        <v>242</v>
+      </c>
+      <c r="G4" s="12">
+        <v>2904</v>
+      </c>
+      <c r="H4" s="12">
+        <v>7944</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>19965</v>
+      </c>
+      <c r="C5" s="12">
+        <v>69615</v>
+      </c>
+      <c r="E5" s="11">
+        <v>4</v>
+      </c>
+      <c r="F5" s="11">
+        <v>266</v>
+      </c>
+      <c r="G5" s="12">
+        <v>3194</v>
+      </c>
+      <c r="H5" s="12">
+        <v>11138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>21961</v>
+      </c>
+      <c r="C6" s="12">
+        <v>91576</v>
+      </c>
+      <c r="E6" s="11">
+        <v>5</v>
+      </c>
+      <c r="F6" s="11">
+        <v>292</v>
+      </c>
+      <c r="G6" s="12">
+        <v>3514</v>
+      </c>
+      <c r="H6" s="12">
+        <v>14652</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>24157</v>
+      </c>
+      <c r="C7" s="12">
+        <v>115733</v>
+      </c>
+      <c r="E7" s="11">
+        <v>6</v>
+      </c>
+      <c r="F7" s="11">
+        <v>321</v>
+      </c>
+      <c r="G7" s="12">
+        <v>3865</v>
+      </c>
+      <c r="H7" s="12">
+        <v>18517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>26573</v>
+      </c>
+      <c r="C8" s="12">
+        <v>142306</v>
+      </c>
+      <c r="E8" s="11">
+        <v>7</v>
+      </c>
+      <c r="F8" s="11">
+        <v>353</v>
+      </c>
+      <c r="G8" s="12">
+        <v>4251</v>
+      </c>
+      <c r="H8" s="12">
+        <v>22768</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12">
+        <v>29230</v>
+      </c>
+      <c r="C9" s="12">
+        <v>171536</v>
+      </c>
+      <c r="E9" s="11">
+        <v>8</v>
+      </c>
+      <c r="F9" s="11">
+        <v>388</v>
+      </c>
+      <c r="G9" s="12">
+        <v>4676</v>
+      </c>
+      <c r="H9" s="12">
+        <v>27444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
+        <v>32153</v>
+      </c>
+      <c r="C10" s="12">
+        <v>203689</v>
+      </c>
+      <c r="E10" s="11">
+        <v>9</v>
+      </c>
+      <c r="F10" s="11">
+        <v>427</v>
+      </c>
+      <c r="G10" s="12">
+        <v>5143</v>
+      </c>
+      <c r="H10" s="12">
+        <v>32587</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12">
+        <v>35368</v>
+      </c>
+      <c r="C11" s="12">
+        <v>239057</v>
+      </c>
+      <c r="E11" s="11">
+        <v>10</v>
+      </c>
+      <c r="F11" s="11">
+        <v>469</v>
+      </c>
+      <c r="G11" s="12">
+        <v>5657</v>
+      </c>
+      <c r="H11" s="12">
+        <v>38244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12">
+        <v>38904</v>
+      </c>
+      <c r="C12" s="12">
+        <v>277961</v>
+      </c>
+      <c r="E12" s="11">
+        <v>11</v>
+      </c>
+      <c r="F12" s="11">
+        <v>516</v>
+      </c>
+      <c r="G12" s="12">
+        <v>6223</v>
+      </c>
+      <c r="H12" s="12">
+        <v>44467</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12">
+        <v>42795</v>
+      </c>
+      <c r="C13" s="12">
+        <v>320756</v>
+      </c>
+      <c r="E13" s="11">
+        <v>12</v>
+      </c>
+      <c r="F13" s="11">
+        <v>567</v>
+      </c>
+      <c r="G13" s="12">
+        <v>6845</v>
+      </c>
+      <c r="H13" s="12">
+        <v>51312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="13">
+        <v>313842</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="E14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="5">
+        <v>50215</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="32" spans="10:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K33" s="3">
+        <v>313842</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="J34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K34" s="3">
+        <v>50215</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="J35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K35" s="3">
+        <v>15600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="J36" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K36" s="5">
+        <v>379657</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F44882-C4E2-4A33-9F29-661429B3153D}">
+  <dimension ref="A1:T15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" customWidth="1"/>
+    <col min="20" max="20" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="E2" s="3">
+        <v>120000</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="2">
+        <v>200</v>
+      </c>
+      <c r="J2" s="2">
+        <v>25</v>
+      </c>
+      <c r="K2" s="3">
+        <v>5000</v>
+      </c>
+      <c r="L2" s="3">
+        <v>60000</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="P2" s="2">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>100</v>
+      </c>
+      <c r="R2" s="2">
+        <v>4</v>
+      </c>
+      <c r="S2" s="3">
+        <v>4000</v>
+      </c>
+      <c r="T2" s="3">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5500</v>
+      </c>
+      <c r="E3" s="3">
+        <v>66000</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="2">
+        <v>100</v>
+      </c>
+      <c r="J3" s="2">
+        <v>70</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" s="3">
+        <v>28000</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P3" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>200</v>
+      </c>
+      <c r="R3" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="S3" s="3">
+        <v>3500</v>
+      </c>
+      <c r="T3" s="3">
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="2">
+        <v>500</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2500</v>
+      </c>
+      <c r="E4" s="3">
+        <v>30000</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="4">
+        <v>300</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P4" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="5">
+        <v>7500</v>
+      </c>
+      <c r="T4" s="5">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="2">
+        <v>500</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2750</v>
+      </c>
+      <c r="E5" s="3">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4000</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="5">
+        <v>20750</v>
+      </c>
+      <c r="E6" s="5">
+        <v>249000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="3">
+        <v>249000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="3">
+        <v>88000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="3">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="5">
+        <v>427000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>